<commit_message>
Final Review Doku & Zeitliste
</commit_message>
<xml_diff>
--- a/Zeitleisten/ESE_Aurednik_Zeitliste.xlsx
+++ b/Zeitleisten/ESE_Aurednik_Zeitliste.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_myCode\net_core\ese.project\Zeitleisten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9495" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Datum</t>
   </si>
@@ -99,9 +99,6 @@
     <t>HTTP Post Mock Recherche</t>
   </si>
   <si>
-    <t>HTTP Post Methode</t>
-  </si>
-  <si>
     <t>HTTP Post Testing und Debugging</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Successful POST without JSMN</t>
   </si>
   <si>
-    <t>Fehlersuche Wiederholter POST  Abbruch</t>
-  </si>
-  <si>
     <t>HW Tests - Lauffähig auf beiden Controllern?</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Dokumentation Embedded Integration</t>
   </si>
   <si>
-    <t>Dokumentation Projektkommunikation</t>
-  </si>
-  <si>
     <t>Projektantrag</t>
   </si>
   <si>
@@ -262,12 +253,45 @@
   </si>
   <si>
     <t>Projektdokumentation Vorlagen konsolidieren</t>
+  </si>
+  <si>
+    <t>Embedded Modulintegration Bewertung</t>
+  </si>
+  <si>
+    <t>Embedded Modulintegration Starting POST from POLL - Debugging</t>
+  </si>
+  <si>
+    <t>Fehlersuche Wiederholter POST  Abbruch - Stackoverflow?</t>
+  </si>
+  <si>
+    <t>Fehlersuche Wiederholter POST  Abbruch - Konfigurationsfehler?</t>
+  </si>
+  <si>
+    <t>Fehlersuche Wiederholter POST  Abbruch - Analyse und Eingrenzung</t>
+  </si>
+  <si>
+    <t>Dokumentation Projektkommunikation - Schreiben</t>
+  </si>
+  <si>
+    <t>Dokumentation Projektkommunikation - Strukturieren</t>
+  </si>
+  <si>
+    <t>Dokumentation Embedded Integration - Strukturieren</t>
+  </si>
+  <si>
+    <t>HTTP Post Mock Recherche - Vergleichen</t>
+  </si>
+  <si>
+    <t>HTTP Post Methode - Selbstimplementierung</t>
+  </si>
+  <si>
+    <t>HTTP Post Methode - Debugging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -723,21 +747,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="8" max="8" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -754,12 +778,12 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>43144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6">
         <v>1.5</v>
@@ -768,7 +792,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43148</v>
       </c>
@@ -779,14 +803,14 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f>SUM(C2:C172)</f>
+        <f>SUM(C2:C178)</f>
         <v>153.5</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43150</v>
       </c>
@@ -800,51 +824,51 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>43150</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43150</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>43150</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43156</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43158</v>
       </c>
@@ -855,29 +879,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>43164</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43164</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43164</v>
       </c>
@@ -888,40 +912,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>43164</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>43164</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>43164</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43164</v>
       </c>
@@ -932,7 +956,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43169</v>
       </c>
@@ -943,29 +967,29 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>43169</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C18" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>43169</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43170</v>
       </c>
@@ -976,29 +1000,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43172</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>43173</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43174</v>
       </c>
@@ -1009,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43174</v>
       </c>
@@ -1020,12 +1044,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>43178</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" s="7">
         <v>2</v>
@@ -1034,7 +1058,7 @@
       <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43178</v>
       </c>
@@ -1048,7 +1072,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43178</v>
       </c>
@@ -1062,23 +1086,23 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>43186</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>43186</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29" s="7">
         <v>0.5</v>
@@ -1087,23 +1111,23 @@
       <c r="H29"/>
       <c r="I29"/>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>43186</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C30" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>43187</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
@@ -1112,7 +1136,7 @@
       <c r="H31"/>
       <c r="I31"/>
     </row>
-    <row r="32" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43189</v>
       </c>
@@ -1123,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43190</v>
       </c>
@@ -1134,12 +1158,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>43200</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C34" s="7">
         <v>0.5</v>
@@ -1148,12 +1172,12 @@
       <c r="H34"/>
       <c r="I34"/>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>43201</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -1162,29 +1186,29 @@
       <c r="H35"/>
       <c r="I35"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43214</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43214</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C37">
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43214</v>
       </c>
@@ -1195,18 +1219,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>43217</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43219</v>
       </c>
@@ -1217,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43219</v>
       </c>
@@ -1228,7 +1252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43219</v>
       </c>
@@ -1239,7 +1263,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43219</v>
       </c>
@@ -1250,34 +1274,34 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43225</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>43229</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>43229</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C46" s="7">
         <v>0.5</v>
@@ -1286,12 +1310,12 @@
       <c r="H46"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>43229</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47" s="7">
         <v>1</v>
@@ -1300,7 +1324,7 @@
       <c r="H47"/>
       <c r="I47"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43237</v>
       </c>
@@ -1311,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43237</v>
       </c>
@@ -1322,18 +1346,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>43240</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C50" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43237</v>
       </c>
@@ -1344,12 +1368,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>43242</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C52" s="7">
         <v>1</v>
@@ -1358,504 +1382,572 @@
       <c r="H52"/>
       <c r="I52"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
         <v>43253</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43255</v>
+        <v>43253</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43255</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43255</v>
       </c>
-      <c r="B56" t="s">
-        <v>25</v>
+      <c r="B56" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43255</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43255</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58">
         <v>1.5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
-        <v>43262</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>43262</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C59" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
-        <v>43272</v>
+        <v>43262</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C60" s="7">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8">
+        <v>43272</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>43274</v>
       </c>
-      <c r="B61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
-        <v>43274</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C62" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>43274</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="C63" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>43274</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8">
+        <v>43274</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43275</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="8">
+        <v>43276</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43276</v>
+      </c>
+      <c r="B68" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="8">
+        <v>43268</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="8">
+        <v>43277</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>43275</v>
-      </c>
-      <c r="B65" t="s">
-        <v>18</v>
-      </c>
-      <c r="C65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>43276</v>
-      </c>
-      <c r="B66" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>43277</v>
-      </c>
-      <c r="B67" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>43278</v>
-      </c>
-      <c r="B68" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>43278</v>
-      </c>
-      <c r="B69" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
-        <v>43268</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
-        <v>43277</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>43280</v>
-      </c>
-      <c r="B72" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>43280</v>
-      </c>
-      <c r="B73" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73">
-        <v>1.5</v>
-      </c>
-      <c r="D73" s="5"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43280</v>
       </c>
       <c r="B74" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C74">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C75">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>43281</v>
-      </c>
-      <c r="B76" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="8">
+        <v>43280</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="7">
+        <v>2</v>
+      </c>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="C77">
-        <v>0.5</v>
-      </c>
-      <c r="D77" s="5"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43281</v>
       </c>
       <c r="B78" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="8">
         <v>43281</v>
       </c>
-      <c r="B79" t="s">
-        <v>36</v>
-      </c>
-      <c r="C79">
-        <v>4</v>
-      </c>
-      <c r="D79" s="5"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43281</v>
       </c>
       <c r="B80" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80" s="5"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43281</v>
       </c>
       <c r="B81" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43281</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C82">
-        <v>1.5</v>
-      </c>
-      <c r="D82" s="5"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
         <v>43281</v>
       </c>
-      <c r="B83" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43281</v>
       </c>
       <c r="B84" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B85" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B86" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B87" t="s">
+        <v>37</v>
+      </c>
+      <c r="C87">
+        <v>1.5</v>
+      </c>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B88" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B90" t="s">
         <v>41</v>
       </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="C90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
         <v>42552</v>
       </c>
-      <c r="B85" t="s">
-        <v>43</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8">
         <v>42552</v>
       </c>
-      <c r="B86" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86">
-        <v>2</v>
-      </c>
-      <c r="D86" s="5"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="B92" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" s="7">
+        <v>1</v>
+      </c>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
         <v>42552</v>
       </c>
-      <c r="B87" t="s">
-        <v>44</v>
-      </c>
-      <c r="C87">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="8">
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="8">
         <v>42552</v>
       </c>
-      <c r="B88" t="s">
-        <v>43</v>
-      </c>
-      <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88" s="5"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8">
-        <v>42553</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
-        <v>42553</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="8">
-        <v>42553</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8">
-        <v>42553</v>
-      </c>
-      <c r="B92" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="8">
-        <v>42553</v>
-      </c>
-      <c r="B93" t="s">
-        <v>62</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
-        <v>42553</v>
-      </c>
       <c r="B94" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C94">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>42553</v>
       </c>
-      <c r="B95" t="s">
-        <v>56</v>
+      <c r="B95" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="C95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>42553</v>
       </c>
-      <c r="B96" t="s">
-        <v>57</v>
+      <c r="B96" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B99" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B101" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="8">
+        <v>42553</v>
+      </c>
+      <c r="B102" t="s">
+        <v>54</v>
+      </c>
+      <c r="C102">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <sortState ref="A2:C12">
+  <sortState ref="A2:C101">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>